<commit_message>
Update docker code and remeasure results
</commit_message>
<xml_diff>
--- a/visualization/data.xlsx
+++ b/visualization/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\now\master_thesis\my_experiment\wasm-docker-comparison\visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542238E5-85F5-4CAB-9BBA-7971F45EA7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7DD06-F0A9-4A90-ABE3-CFE7A22B206B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B2AD0577-FAA7-4A8A-8625-21F998F05787}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2AD0577-FAA7-4A8A-8625-21F998F05787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,14 +449,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF328FB-343A-4F51-9621-F549EA9A7AC6}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
@@ -504,25 +504,25 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>3.6242999999999997E-2</v>
+        <v>4.0315000000000004E-2</v>
       </c>
       <c r="D2">
-        <v>0.36278700000000008</v>
+        <v>0.37406200000000001</v>
       </c>
       <c r="E2">
-        <v>2.0819999999999998E-2</v>
+        <v>1.7547E-2</v>
       </c>
       <c r="F2">
-        <v>0.42508400000000002</v>
+        <v>0.43670199999999992</v>
       </c>
       <c r="G2">
-        <v>1.9335899999999999</v>
+        <v>561.73690800000008</v>
       </c>
       <c r="H2">
-        <v>0.70710959060000023</v>
+        <v>0.76539985170000002</v>
       </c>
       <c r="I2">
-        <v>97.803408999999988</v>
+        <v>98.462383000000003</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -533,25 +533,25 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>0.12692200000000001</v>
+        <v>0.14466099999999998</v>
       </c>
       <c r="D3">
-        <v>5.8580829999999997</v>
+        <v>5.5420719999999992</v>
       </c>
       <c r="E3">
-        <v>6.9387000000000004E-2</v>
+        <v>6.7990000000000009E-2</v>
       </c>
       <c r="F3">
-        <v>6.0592220000000001</v>
+        <v>5.7593580000000006</v>
       </c>
       <c r="G3">
-        <v>7.7605460000000006</v>
+        <v>565.30042800000012</v>
       </c>
       <c r="H3">
-        <v>0.72110187400000081</v>
+        <v>0.77416018910000017</v>
       </c>
       <c r="I3">
-        <v>99.391600000000011</v>
+        <v>99.598020999999989</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -562,25 +562,25 @@
         <v>1500</v>
       </c>
       <c r="C4">
-        <v>0.265594</v>
+        <v>0.29814200000000002</v>
       </c>
       <c r="D4">
-        <v>26.195297999999998</v>
+        <v>25.746622000000002</v>
       </c>
       <c r="E4">
-        <v>0.14696599999999999</v>
+        <v>0.14802100000000001</v>
       </c>
       <c r="F4">
-        <v>26.612837000000003</v>
+        <v>26.197103999999996</v>
       </c>
       <c r="G4">
-        <v>17.285159999999998</v>
+        <v>575.30367999999999</v>
       </c>
       <c r="H4">
-        <v>0.75510829629999543</v>
+        <v>0.81716950510000286</v>
       </c>
       <c r="I4">
-        <v>99.974165999999997</v>
+        <v>99.126615999999984</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -591,25 +591,25 @@
         <v>2000</v>
       </c>
       <c r="C5">
-        <v>0.47291300000000003</v>
+        <v>0.51958900000000008</v>
       </c>
       <c r="D5">
-        <v>81.907958999999991</v>
+        <v>79.709877999999989</v>
       </c>
       <c r="E5">
-        <v>0.25451499999999994</v>
+        <v>0.26037199999999999</v>
       </c>
       <c r="F5">
-        <v>82.640192999999996</v>
+        <v>80.49410499999999</v>
       </c>
       <c r="G5">
-        <v>30.652339999999999</v>
+        <v>589.32019000000014</v>
       </c>
       <c r="H5">
-        <v>0.76462612250000883</v>
+        <v>0.77876618349999982</v>
       </c>
       <c r="I5">
-        <v>99.997462999999996</v>
+        <v>99.382960999999995</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -620,25 +620,25 @@
         <v>2500</v>
       </c>
       <c r="C6">
-        <v>1.0756459999999999</v>
+        <v>0.88073699999999988</v>
       </c>
       <c r="D6">
-        <v>193.769904</v>
+        <v>164.71641100000002</v>
       </c>
       <c r="E6">
-        <v>0.42558499999999999</v>
+        <v>0.38848999999999995</v>
       </c>
       <c r="F6">
-        <v>195.27605700000001</v>
+        <v>165.99040000000002</v>
       </c>
       <c r="G6">
-        <v>112.03906000000003</v>
+        <v>654.527692</v>
       </c>
       <c r="H6">
-        <v>0.83125661249999272</v>
+        <v>0.89868549099998052</v>
       </c>
       <c r="I6">
-        <v>99.984476999999998</v>
+        <v>99.359617</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -649,25 +649,25 @@
         <v>3000</v>
       </c>
       <c r="C7">
-        <v>2.3716849999999998</v>
+        <v>1.2209080000000001</v>
       </c>
       <c r="D7">
-        <v>366.851586</v>
+        <v>292.67709000000002</v>
       </c>
       <c r="E7">
-        <v>0.63888099999999992</v>
+        <v>0.54593100000000006</v>
       </c>
       <c r="F7">
-        <v>369.86742800000002</v>
+        <v>294.449051</v>
       </c>
       <c r="G7">
-        <v>132.92187999999996</v>
+        <v>676.42490900000007</v>
       </c>
       <c r="H7">
-        <v>1.3368123351999568</v>
+        <v>0.8933892905999905</v>
       </c>
       <c r="I7">
-        <v>99.986815000000007</v>
+        <v>99.145011000000011</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -678,25 +678,25 @@
         <v>3500</v>
       </c>
       <c r="C8">
-        <v>1.5446880000000001</v>
+        <v>1.6298109999999997</v>
       </c>
       <c r="D8">
-        <v>451.09423699999996</v>
+        <v>456.05521099999999</v>
       </c>
       <c r="E8">
-        <v>0.78377699999999995</v>
+        <v>0.76395399999999991</v>
       </c>
       <c r="F8">
-        <v>453.42816899999997</v>
+        <v>458.45398399999993</v>
       </c>
       <c r="G8">
-        <v>157.74609000000004</v>
+        <v>689.03321500000015</v>
       </c>
       <c r="H8">
-        <v>0.96413909149996957</v>
+        <v>1.2263776955000567</v>
       </c>
       <c r="I8">
-        <v>99.520223000000001</v>
+        <v>99.561093</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -707,25 +707,25 @@
         <v>4000</v>
       </c>
       <c r="C9">
-        <v>2.0708049999999996</v>
+        <v>2.2749229999999998</v>
       </c>
       <c r="D9">
-        <v>659.93451299999992</v>
+        <v>661.21831399999996</v>
       </c>
       <c r="E9">
-        <v>1.161934</v>
+        <v>1.1561399999999999</v>
       </c>
       <c r="F9">
-        <v>663.17204800000002</v>
+        <v>664.7468922999999</v>
       </c>
       <c r="G9">
-        <v>186.35937999999996</v>
+        <v>719.03641500000015</v>
       </c>
       <c r="H9">
-        <v>0.92969473849993578</v>
+        <v>1.1345237217002104</v>
       </c>
       <c r="I9">
-        <v>99.475270999999992</v>
+        <v>99.450023999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -736,25 +736,25 @@
         <v>4500</v>
       </c>
       <c r="C10">
-        <v>5.364859</v>
+        <v>3.2225139999999994</v>
       </c>
       <c r="D10">
-        <v>1071.121181</v>
+        <v>1014.477743</v>
       </c>
       <c r="E10">
-        <v>1.9334479999999998</v>
+        <v>1.7799119999999999</v>
       </c>
       <c r="F10">
-        <v>1078.4246410000001</v>
+        <v>1019.4852539999999</v>
       </c>
       <c r="G10">
-        <v>218.82422000000003</v>
+        <v>753.07826999999997</v>
       </c>
       <c r="H10">
-        <v>1.1607037810998415</v>
+        <v>1.0610198906998869</v>
       </c>
       <c r="I10">
-        <v>99.554563000000002</v>
+        <v>99.444389000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -765,25 +765,25 @@
         <v>5000</v>
       </c>
       <c r="C11">
-        <v>5.2999290000000006</v>
+        <v>4.4215290000000005</v>
       </c>
       <c r="D11">
-        <v>1466.4175770000002</v>
+        <v>1351.746848</v>
       </c>
       <c r="E11">
-        <v>2.615367</v>
+        <v>2.4355809999999996</v>
       </c>
       <c r="F11">
-        <v>1474.338452</v>
+        <v>1358.6087310000003</v>
       </c>
       <c r="G11">
-        <v>255.07031000000001</v>
+        <v>791.0850549999999</v>
       </c>
       <c r="H11">
-        <v>1.123237702399918</v>
+        <v>1.1303745282995989</v>
       </c>
       <c r="I11">
-        <v>99.552760000000006</v>
+        <v>99.581677999999997</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -794,25 +794,25 @@
         <v>5500</v>
       </c>
       <c r="C12">
-        <v>6.0821489999999994</v>
+        <v>6.5283230000000003</v>
       </c>
       <c r="D12">
-        <v>2113.7681010000001</v>
+        <v>1926.9737460000001</v>
       </c>
       <c r="E12">
-        <v>3.1921010000000001</v>
+        <v>3.0917139999999996</v>
       </c>
       <c r="F12">
-        <v>2123.0480210000001</v>
+        <v>1936.5988019999998</v>
       </c>
       <c r="G12">
-        <v>295.13672000000003</v>
+        <v>846.51950199999987</v>
       </c>
       <c r="H12">
-        <v>1.2846877698999699</v>
+        <v>1.1106633383001581</v>
       </c>
       <c r="I12">
-        <v>99.729159999999993</v>
+        <v>99.683218000000011</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>